<commit_message>
updating styling and alumni
</commit_message>
<xml_diff>
--- a/src/data/alumni.xlsx
+++ b/src/data/alumni.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Website Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02DDA8C-8081-4F89-8F31-66EEFC113476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6A16CA3-1FEB-429C-AD34-A35B7A3F0761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="3870" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alumni" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t>name1</t>
   </si>
@@ -142,12 +142,6 @@
     <t>https://www.linkedin.com/in/manroop-gill/</t>
   </si>
   <si>
-    <t>Jason Van</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/jason-van/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alexander McGuigan </t>
   </si>
   <si>
@@ -238,12 +232,6 @@
     <t>https://www.linkedin.com/in/parm-sidhu/</t>
   </si>
   <si>
-    <t>Beverley Fung</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/beverleyfung/</t>
-  </si>
-  <si>
     <t>Miguel Valarao</t>
   </si>
   <si>
@@ -271,12 +259,6 @@
     <t>https://www.linkedin.com/in/nicholaseverett/</t>
   </si>
   <si>
-    <t>David Buzza</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/davidbuzza/</t>
-  </si>
-  <si>
     <t>Christian Bernad</t>
   </si>
   <si>
@@ -386,12 +368,6 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/sunnyshee/</t>
-  </si>
-  <si>
-    <t>Pranoy Debnath</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/pranoy-debnath-pd/</t>
   </si>
   <si>
     <t>Gurman Sihota</t>
@@ -780,8 +756,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -902,10 +878,10 @@
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
@@ -922,10 +898,10 @@
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>32</v>
@@ -936,16 +912,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>38</v>
@@ -956,70 +932,70 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>75</v>
@@ -1028,18 +1004,18 @@
         <v>76</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>79</v>
@@ -1048,58 +1024,58 @@
         <v>80</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>93</v>
@@ -1108,58 +1084,58 @@
         <v>94</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>106</v>
@@ -1168,150 +1144,124 @@
         <v>107</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>152</v>
+        <v>134</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1341,64 +1291,60 @@
     <hyperlink ref="B7" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="D5" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="F8" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B8" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D6" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F9" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B9" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F10" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B10" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D8" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F11" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B11" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D9" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F12" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B12" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D10" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F13" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B13" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D11" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D12" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="F15" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D13" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="F16" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B14" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D14" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="F17" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D15" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="F18" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="D16" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="F19" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B15" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D17" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D18" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="F21" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D19" r:id="rId50" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="F22" r:id="rId51" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B16" r:id="rId52" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="D20" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="F23" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B17" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B21" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="F24" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B18" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B22" r:id="rId59" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="F25" r:id="rId60" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B23" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D24" r:id="rId62" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B26" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B19" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D25" r:id="rId65" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D21" r:id="rId66" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B25" r:id="rId67" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D26" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="D23" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B24" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="F14" r:id="rId71" xr:uid="{D69414DC-110E-44F3-A34A-FA8B122A1848}"/>
-    <hyperlink ref="F20" r:id="rId72" xr:uid="{1238A2ED-70BA-49AD-9ABF-CF9C731AA064}"/>
-    <hyperlink ref="F26" r:id="rId73" xr:uid="{141F7BAF-BDB6-4D89-9E07-587DD4CA8189}"/>
-    <hyperlink ref="D22" r:id="rId74" xr:uid="{B4CBA527-4E11-45F6-AB16-5841A661A150}"/>
-    <hyperlink ref="B20" r:id="rId75" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="D6" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B8" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D7" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F10" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B9" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D8" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F11" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B10" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D9" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F12" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B11" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D10" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F13" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B12" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D11" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F15" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D12" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F16" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D13" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F17" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D14" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F18" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D15" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F19" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B13" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D16" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D17" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F21" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="D18" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F22" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B14" r:id="rId49" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="D19" r:id="rId50" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F23" r:id="rId51" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B15" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B18" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F24" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B19" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F25" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B20" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D23" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B23" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B16" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D24" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D20" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B22" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D25" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="D22" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B21" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F14" r:id="rId67" xr:uid="{D69414DC-110E-44F3-A34A-FA8B122A1848}"/>
+    <hyperlink ref="F20" r:id="rId68" xr:uid="{1238A2ED-70BA-49AD-9ABF-CF9C731AA064}"/>
+    <hyperlink ref="B24" r:id="rId69" xr:uid="{141F7BAF-BDB6-4D89-9E07-587DD4CA8189}"/>
+    <hyperlink ref="D21" r:id="rId70" xr:uid="{B4CBA527-4E11-45F6-AB16-5841A661A150}"/>
+    <hyperlink ref="B17" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated alumni and hiring
</commit_message>
<xml_diff>
--- a/src/data/alumni.xlsx
+++ b/src/data/alumni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jocelyn/Desktop/WestPeak/git/WestPeakWebsite/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13B8DA0-F211-7F46-9D6E-3E015BEFE268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C2E4BD-8CB3-8246-A51C-C7E736B09126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="172">
   <si>
     <t>name1</t>
   </si>
@@ -487,12 +487,6 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/hasanaltaf/</t>
-  </si>
-  <si>
-    <t>Irene Liu</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ireneqliu/</t>
   </si>
   <si>
     <t>Jake Bunderla</t>
@@ -874,8 +868,8 @@
   </sheetPr>
   <dimension ref="A1:F1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -936,70 +930,70 @@
         <v>153</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>167</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>173</v>
+        <v>169</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
@@ -1016,10 +1010,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>16</v>
@@ -1036,10 +1030,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>22</v>
@@ -1056,10 +1050,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>28</v>
@@ -1076,10 +1070,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>34</v>
@@ -1096,10 +1090,10 @@
         <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>40</v>
@@ -1116,10 +1110,10 @@
         <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>46</v>
@@ -1136,10 +1130,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>52</v>
@@ -1156,10 +1150,10 @@
         <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>58</v>
@@ -1176,10 +1170,10 @@
         <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>64</v>
@@ -1196,10 +1190,10 @@
         <v>61</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>70</v>
@@ -1216,10 +1210,10 @@
         <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>76</v>
@@ -1236,10 +1230,10 @@
         <v>73</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>82</v>
@@ -1256,10 +1250,10 @@
         <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>87</v>
@@ -1276,10 +1270,10 @@
         <v>84</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>93</v>
@@ -1296,10 +1290,10 @@
         <v>90</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>99</v>
@@ -1316,10 +1310,10 @@
         <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>105</v>
@@ -1336,10 +1330,10 @@
         <v>102</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>111</v>
@@ -1356,10 +1350,10 @@
         <v>108</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>117</v>
@@ -1375,11 +1369,11 @@
       <c r="B25" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>116</v>
+      <c r="C25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>121</v>
@@ -1395,11 +1389,11 @@
       <c r="B26" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>23</v>
+      <c r="C26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>127</v>
@@ -1416,10 +1410,10 @@
         <v>124</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>133</v>
@@ -1436,10 +1430,10 @@
         <v>130</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>138</v>
@@ -1456,10 +1450,10 @@
         <v>23</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>144</v>
@@ -1474,12 +1468,6 @@
       </c>
       <c r="B30" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2460,91 +2448,90 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="F9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="F10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="B12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="F11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="B13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D12" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="F12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="B14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D14" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
     <hyperlink ref="F13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="B15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D15" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="F14" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="B16" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D15" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="F15" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="B17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D16" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="F16" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="B18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D18" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D17" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="F17" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
     <hyperlink ref="B19" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D19" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D18" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
     <hyperlink ref="F18" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
     <hyperlink ref="B20" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D20" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D19" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
     <hyperlink ref="F19" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
     <hyperlink ref="B21" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D21" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D20" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
     <hyperlink ref="F20" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="B22" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D22" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D21" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="F21" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="B23" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D23" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D22" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
     <hyperlink ref="F22" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
     <hyperlink ref="B24" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D24" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D23" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
     <hyperlink ref="F23" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
     <hyperlink ref="B25" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D25" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="D24" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="F24" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="B26" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D26" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="D25" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
     <hyperlink ref="F25" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
     <hyperlink ref="B27" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D27" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="D26" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
     <hyperlink ref="F26" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
     <hyperlink ref="B28" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D28" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D27" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="F27" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
     <hyperlink ref="B29" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="D29" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D28" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
     <hyperlink ref="F28" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
     <hyperlink ref="B30" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="D30" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D29" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
     <hyperlink ref="F29" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D6" r:id="rId73" xr:uid="{66AB4C4E-9860-FA48-B2C8-DB08F1F73178}"/>
+    <hyperlink ref="D5" r:id="rId73" xr:uid="{66AB4C4E-9860-FA48-B2C8-DB08F1F73178}"/>
     <hyperlink ref="B6" r:id="rId74" xr:uid="{827C436A-A44F-EF4C-BCCA-546A6ABD4868}"/>
     <hyperlink ref="F5" r:id="rId75" xr:uid="{DEEB2C52-D2A5-0040-A025-C1E605BFFBD6}"/>
-    <hyperlink ref="D5" r:id="rId76" xr:uid="{94C05838-6EC9-F44F-B317-B694BAF81186}"/>
+    <hyperlink ref="D4" r:id="rId76" xr:uid="{94C05838-6EC9-F44F-B317-B694BAF81186}"/>
     <hyperlink ref="B5" r:id="rId77" xr:uid="{2022A4ED-DEAA-404D-B8EA-46FA4E5185D2}"/>
     <hyperlink ref="F4" r:id="rId78" xr:uid="{E0B5A9D8-932F-C24A-89CB-52A16898A96C}"/>
-    <hyperlink ref="D4" r:id="rId79" xr:uid="{27C7D2C4-D927-164B-9BE5-34D2F98AE2B0}"/>
+    <hyperlink ref="D3" r:id="rId79" xr:uid="{27C7D2C4-D927-164B-9BE5-34D2F98AE2B0}"/>
     <hyperlink ref="B4" r:id="rId80" xr:uid="{6D397E78-9C11-A94C-A41A-D062E4D01F4F}"/>
     <hyperlink ref="F3" r:id="rId81" xr:uid="{3102F2EF-9BF2-BC4F-ABE5-EE9F651363F8}"/>
-    <hyperlink ref="D3" r:id="rId82" xr:uid="{93A42605-6CC3-714B-A0CC-03813E94B709}"/>
-    <hyperlink ref="B3" r:id="rId83" xr:uid="{C52691DB-0D6A-864C-9679-7CAB01CA9E14}"/>
-    <hyperlink ref="F2" r:id="rId84" xr:uid="{6F3472D8-4628-3940-B552-7F6C5967534D}"/>
-    <hyperlink ref="D2" r:id="rId85" xr:uid="{BF6AAD05-C343-6347-B777-0AC78CFD523D}"/>
-    <hyperlink ref="B2" r:id="rId86" xr:uid="{F2373978-DBDC-7A4D-8B3D-EDD5D8F3F47F}"/>
+    <hyperlink ref="B3" r:id="rId82" xr:uid="{C52691DB-0D6A-864C-9679-7CAB01CA9E14}"/>
+    <hyperlink ref="F2" r:id="rId83" xr:uid="{6F3472D8-4628-3940-B552-7F6C5967534D}"/>
+    <hyperlink ref="D2" r:id="rId84" xr:uid="{BF6AAD05-C343-6347-B777-0AC78CFD523D}"/>
+    <hyperlink ref="B2" r:id="rId85" xr:uid="{F2373978-DBDC-7A4D-8B3D-EDD5D8F3F47F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Update team and alumni
</commit_message>
<xml_diff>
--- a/src/data/alumni.xlsx
+++ b/src/data/alumni.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jocelyn/Desktop/WestPeak/git/WestPeakWebsite/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BEF29-4385-3F47-AD50-4EC15C9E9450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C7C1D7-A84C-1445-A5D7-A3E27797AD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="25600" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="182">
   <si>
     <t>name1</t>
   </si>
@@ -513,12 +513,6 @@
     <t>https://www.linkedin.com/in/samuelalchen/</t>
   </si>
   <si>
-    <t>Surav Malla</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/surav-malla/</t>
-  </si>
-  <si>
     <t>Szarri Lim</t>
   </si>
   <si>
@@ -541,13 +535,49 @@
   </si>
   <si>
     <t>Matthew West</t>
+  </si>
+  <si>
+    <t>Dylan Assi</t>
+  </si>
+  <si>
+    <t>Simrit Hundal</t>
+  </si>
+  <si>
+    <t>Gurnoor Minhas</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/simrithundal/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/gurnoorkm/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dylanassi/</t>
+  </si>
+  <si>
+    <t>Davis Li</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/davisli1/</t>
+  </si>
+  <si>
+    <t>Jessica Zhang</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jessicazrzhang/</t>
+  </si>
+  <si>
+    <t>Irene Liu</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ireneqliu/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -587,6 +617,12 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -623,7 +659,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,17 +672,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -869,17 +905,17 @@
   <dimension ref="A1:F1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C7" sqref="C7:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="42.5" style="10" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="45.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
-    <col min="6" max="6" width="45.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="45.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -903,575 +939,613 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>165</v>
+      <c r="D5" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>167</v>
+      <c r="A6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>156</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>11</v>
+        <v>158</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>154</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>166</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>17</v>
+        <v>162</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
+        <v>160</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>164</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>171</v>
+        <v>52</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>23</v>
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>93</v>
+        <v>80</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>23</v>
+        <v>103</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>23</v>
+        <v>101</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>127</v>
+        <v>115</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>131</v>
+        <v>113</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C31" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2447,91 +2521,97 @@
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B13" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D12" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B14" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="F13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B15" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F14" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B16" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D15" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F15" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D16" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F16" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D17" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F17" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B19" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D18" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F18" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B20" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D19" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="F19" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B21" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D20" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F20" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B22" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D21" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="F21" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B23" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D22" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="F22" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B24" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="D23" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="F23" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B25" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D24" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="F24" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B26" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D25" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="F25" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B27" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D26" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="F26" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B28" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="D27" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="F27" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B29" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="D28" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="F28" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B30" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="D29" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F29" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D5" r:id="rId73" xr:uid="{66AB4C4E-9860-FA48-B2C8-DB08F1F73178}"/>
-    <hyperlink ref="B6" r:id="rId74" xr:uid="{827C436A-A44F-EF4C-BCCA-546A6ABD4868}"/>
-    <hyperlink ref="F5" r:id="rId75" xr:uid="{DEEB2C52-D2A5-0040-A025-C1E605BFFBD6}"/>
-    <hyperlink ref="D4" r:id="rId76" xr:uid="{94C05838-6EC9-F44F-B317-B694BAF81186}"/>
-    <hyperlink ref="B5" r:id="rId77" xr:uid="{2022A4ED-DEAA-404D-B8EA-46FA4E5185D2}"/>
-    <hyperlink ref="F4" r:id="rId78" xr:uid="{E0B5A9D8-932F-C24A-89CB-52A16898A96C}"/>
-    <hyperlink ref="D3" r:id="rId79" xr:uid="{27C7D2C4-D927-164B-9BE5-34D2F98AE2B0}"/>
-    <hyperlink ref="B4" r:id="rId80" xr:uid="{6D397E78-9C11-A94C-A41A-D062E4D01F4F}"/>
-    <hyperlink ref="F3" r:id="rId81" xr:uid="{3102F2EF-9BF2-BC4F-ABE5-EE9F651363F8}"/>
-    <hyperlink ref="B3" r:id="rId82" xr:uid="{C52691DB-0D6A-864C-9679-7CAB01CA9E14}"/>
-    <hyperlink ref="F2" r:id="rId83" xr:uid="{6F3472D8-4628-3940-B552-7F6C5967534D}"/>
-    <hyperlink ref="D2" r:id="rId84" xr:uid="{BF6AAD05-C343-6347-B777-0AC78CFD523D}"/>
-    <hyperlink ref="B2" r:id="rId85" xr:uid="{F2373978-DBDC-7A4D-8B3D-EDD5D8F3F47F}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B15" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F14" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B16" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F15" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B17" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D16" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F16" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B18" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D17" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F17" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B19" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D18" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F18" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B20" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D19" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B21" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B22" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F21" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B23" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D22" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F22" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D23" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F23" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B25" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D24" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F24" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B26" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="D25" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F25" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B27" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D26" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F26" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B28" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="D27" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F27" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B29" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D28" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F28" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B30" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D29" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F29" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B31" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="D30" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F30" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D31" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B32" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F31" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D7" r:id="rId72" xr:uid="{66AB4C4E-9860-FA48-B2C8-DB08F1F73178}"/>
+    <hyperlink ref="B9" r:id="rId73" xr:uid="{827C436A-A44F-EF4C-BCCA-546A6ABD4868}"/>
+    <hyperlink ref="F7" r:id="rId74" xr:uid="{DEEB2C52-D2A5-0040-A025-C1E605BFFBD6}"/>
+    <hyperlink ref="B8" r:id="rId75" xr:uid="{2022A4ED-DEAA-404D-B8EA-46FA4E5185D2}"/>
+    <hyperlink ref="F6" r:id="rId76" xr:uid="{E0B5A9D8-932F-C24A-89CB-52A16898A96C}"/>
+    <hyperlink ref="D6" r:id="rId77" xr:uid="{27C7D2C4-D927-164B-9BE5-34D2F98AE2B0}"/>
+    <hyperlink ref="B7" r:id="rId78" xr:uid="{6D397E78-9C11-A94C-A41A-D062E4D01F4F}"/>
+    <hyperlink ref="F5" r:id="rId79" xr:uid="{3102F2EF-9BF2-BC4F-ABE5-EE9F651363F8}"/>
+    <hyperlink ref="B6" r:id="rId80" xr:uid="{C52691DB-0D6A-864C-9679-7CAB01CA9E14}"/>
+    <hyperlink ref="F4" r:id="rId81" xr:uid="{6F3472D8-4628-3940-B552-7F6C5967534D}"/>
+    <hyperlink ref="D5" r:id="rId82" xr:uid="{BF6AAD05-C343-6347-B777-0AC78CFD523D}"/>
+    <hyperlink ref="B5" r:id="rId83" xr:uid="{F2373978-DBDC-7A4D-8B3D-EDD5D8F3F47F}"/>
+    <hyperlink ref="B2" r:id="rId84" xr:uid="{5760081B-7AF4-3B40-8DCF-8A0ADF761C6F}"/>
+    <hyperlink ref="F2" r:id="rId85" xr:uid="{CAD19926-6DAE-A64B-9B8C-6BDA6F6D4BE1}"/>
+    <hyperlink ref="D2" r:id="rId86" xr:uid="{C38A4477-6070-EE48-B801-E7570435858C}"/>
+    <hyperlink ref="B3" r:id="rId87" xr:uid="{28FFC515-DE9F-FE45-B437-273AEFC0D408}"/>
+    <hyperlink ref="D3" r:id="rId88" xr:uid="{C7A563D3-1A36-4E44-BFE0-25DF4861C3F4}"/>
+    <hyperlink ref="F3" r:id="rId89" xr:uid="{3E883737-2498-CF48-A751-0AECE0BE7507}"/>
+    <hyperlink ref="B4" r:id="rId90" xr:uid="{42281DCF-ACAA-7045-B73A-CD3919A44931}"/>
+    <hyperlink ref="D4" r:id="rId91" xr:uid="{08AF3101-B4C6-E544-ABB5-91800BDA40A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>